<commit_message>
[MS-SHDACCWS] Update RS according to lastest version TD
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-SHDACCWS/MS-SHDACCWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-SHDACCWS/MS-SHDACCWS_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="173">
   <si>
     <t>Req ID</t>
   </si>
@@ -800,20 +800,24 @@
 Implementation does additionally support SOAP over HTTPS for securing communication with clients.
 (Microsoft SharePoint Foundation 2010, Microsoft SharePoint Foundation 2013 and Microsoft SharePoint Server 2016 products follow this behavior.)</t>
   </si>
+  <si>
+    <t>Unverified</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1009,13 +1013,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1048,7 +1052,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1069,21 +1073,6 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1108,6 +1097,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1775,7 +1779,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1808,9 +1812,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1843,6 +1864,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2022,26 +2060,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="20.625" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>167</v>
       </c>
@@ -2051,7 +2087,7 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>168</v>
       </c>
@@ -2062,7 +2098,7 @@
       <c r="F2" s="25"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
@@ -2077,131 +2113,131 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="78.75" customHeight="1">
+    <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="33.75" customHeight="1">
+    <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
@@ -2211,15 +2247,15 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
@@ -2229,15 +2265,15 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>7</v>
       </c>
@@ -2247,15 +2283,15 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>3</v>
       </c>
@@ -2265,64 +2301,64 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1">
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="64.5" customHeight="1">
+    <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -2352,7 +2388,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1">
+    <row r="20" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="22" t="s">
         <v>42</v>
       </c>
@@ -2377,7 +2413,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A21" s="22" t="s">
         <v>43</v>
       </c>
@@ -2404,7 +2440,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="75">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A22" s="22" t="s">
         <v>44</v>
       </c>
@@ -2433,7 +2469,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="23" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A23" s="22" t="s">
         <v>45</v>
       </c>
@@ -2458,7 +2494,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A24" s="22" t="s">
         <v>46</v>
       </c>
@@ -2479,11 +2515,11 @@
         <v>15</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>21</v>
+        <v>172</v>
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="25" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="22" t="s">
         <v>47</v>
       </c>
@@ -2508,7 +2544,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="26" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A26" s="22" t="s">
         <v>48</v>
       </c>
@@ -2533,7 +2569,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="27" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A27" s="22" t="s">
         <v>49</v>
       </c>
@@ -2558,7 +2594,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A28" s="22" t="s">
         <v>50</v>
       </c>
@@ -2583,7 +2619,7 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A29" s="22" t="s">
         <v>51</v>
       </c>
@@ -2608,7 +2644,7 @@
       </c>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="30" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A30" s="22" t="s">
         <v>52</v>
       </c>
@@ -2633,7 +2669,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A31" s="22" t="s">
         <v>53</v>
       </c>
@@ -2658,7 +2694,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="32" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A32" s="22" t="s">
         <v>54</v>
       </c>
@@ -2683,7 +2719,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" ht="30">
+    <row r="33" spans="1:9" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A33" s="22" t="s">
         <v>55</v>
       </c>
@@ -2708,7 +2744,7 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" ht="30">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>56</v>
       </c>
@@ -2733,7 +2769,7 @@
       </c>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" ht="30">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
         <v>57</v>
       </c>
@@ -2758,7 +2794,7 @@
       </c>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" ht="30">
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>58</v>
       </c>
@@ -2783,7 +2819,7 @@
       </c>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" ht="30">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>59</v>
       </c>
@@ -2808,7 +2844,7 @@
       </c>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9" ht="30">
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
         <v>60</v>
       </c>
@@ -2833,7 +2869,7 @@
       </c>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" ht="30">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>61</v>
       </c>
@@ -2858,7 +2894,7 @@
       </c>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
         <v>62</v>
       </c>
@@ -2883,7 +2919,7 @@
       </c>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" ht="30">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>63</v>
       </c>
@@ -2908,7 +2944,7 @@
       </c>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" ht="45">
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>64</v>
       </c>
@@ -2933,7 +2969,7 @@
       </c>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" ht="45">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
         <v>65</v>
       </c>
@@ -2958,7 +2994,7 @@
       </c>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9" ht="30">
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
         <v>66</v>
       </c>
@@ -2983,7 +3019,7 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="45">
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
         <v>67</v>
       </c>
@@ -3008,7 +3044,7 @@
       </c>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" ht="45">
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
         <v>68</v>
       </c>
@@ -3033,7 +3069,7 @@
       </c>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" ht="30">
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
         <v>69</v>
       </c>
@@ -3058,7 +3094,7 @@
       </c>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" spans="1:9" ht="30">
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
         <v>70</v>
       </c>
@@ -3083,7 +3119,7 @@
       </c>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" ht="30">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>71</v>
       </c>
@@ -3108,7 +3144,7 @@
       </c>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" ht="75">
+    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>72</v>
       </c>
@@ -3133,7 +3169,7 @@
       </c>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
         <v>73</v>
       </c>
@@ -3158,7 +3194,7 @@
       </c>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="30">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
         <v>74</v>
       </c>
@@ -3183,7 +3219,7 @@
       </c>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" ht="30">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
         <v>75</v>
       </c>
@@ -3208,7 +3244,7 @@
       </c>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" ht="30">
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="30" t="s">
         <v>76</v>
       </c>
@@ -3233,7 +3269,7 @@
       </c>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="30" t="s">
         <v>77</v>
       </c>
@@ -3258,7 +3294,7 @@
       </c>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="30" t="s">
         <v>78</v>
       </c>
@@ -3283,7 +3319,7 @@
       </c>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="30" t="s">
         <v>79</v>
       </c>
@@ -3308,7 +3344,7 @@
       </c>
       <c r="I57" s="32"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="30" t="s">
         <v>80</v>
       </c>
@@ -3333,7 +3369,7 @@
       </c>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="30" t="s">
         <v>81</v>
       </c>
@@ -3358,7 +3394,7 @@
       </c>
       <c r="I59" s="32"/>
     </row>
-    <row r="60" spans="1:9" ht="30">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
         <v>82</v>
       </c>
@@ -3383,7 +3419,7 @@
       </c>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" ht="45">
+    <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
         <v>83</v>
       </c>
@@ -3408,7 +3444,7 @@
       </c>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="30">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>84</v>
       </c>
@@ -3433,7 +3469,7 @@
       </c>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:9" ht="135">
+    <row r="63" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
         <v>85</v>
       </c>
@@ -3458,7 +3494,7 @@
       </c>
       <c r="I63" s="32"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
         <v>86</v>
       </c>
@@ -3483,7 +3519,7 @@
       </c>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" ht="150">
+    <row r="65" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
         <v>87</v>
       </c>
@@ -3508,7 +3544,7 @@
       </c>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
         <v>88</v>
       </c>
@@ -3533,7 +3569,7 @@
       </c>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" ht="135">
+    <row r="67" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
         <v>89</v>
       </c>
@@ -3558,7 +3594,7 @@
       </c>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" ht="30">
+    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
         <v>90</v>
       </c>
@@ -3583,7 +3619,7 @@
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="75">
+    <row r="69" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>91</v>
       </c>
@@ -3610,7 +3646,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
         <v>92</v>
       </c>
@@ -3637,7 +3673,7 @@
       </c>
       <c r="I70" s="32"/>
     </row>
-    <row r="71" spans="1:9" ht="30">
+    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
         <v>93</v>
       </c>
@@ -3664,7 +3700,7 @@
       </c>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>94</v>
       </c>
@@ -3691,7 +3727,7 @@
       </c>
       <c r="I72" s="32"/>
     </row>
-    <row r="73" spans="1:9" ht="45">
+    <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
         <v>95</v>
       </c>
@@ -3716,7 +3752,7 @@
       </c>
       <c r="I73" s="32"/>
     </row>
-    <row r="74" spans="1:9" ht="30">
+    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
         <v>96</v>
       </c>
@@ -3741,16 +3777,21 @@
       </c>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="10"/>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -3758,11 +3799,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A71:B71 A20:H70 A34:I70 A72:I74 D71:I71">
@@ -3873,18 +3909,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3937,6 +3973,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3946,14 +3990,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update Open Specification Version and Standardize RS for MS-ADMINS, MS-CPSWS, MS-SHDACCWS and MS-WEBSS.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-SHDACCWS/MS-SHDACCWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-SHDACCWS/MS-SHDACCWS_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="174">
   <si>
     <t>Req ID</t>
   </si>
@@ -804,6 +804,10 @@
     <t>Unverified</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>6.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -857,6 +861,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1062,9 +1067,6 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1073,6 +1075,24 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1097,21 +1117,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2064,7 +2069,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
@@ -2102,8 +2107,8 @@
       <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="29">
-        <v>6</v>
+      <c r="C3" s="32" t="s">
+        <v>173</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>170</v>
@@ -2114,127 +2119,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2247,12 +2252,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2265,12 +2270,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2283,12 +2288,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2301,60 +2306,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -2745,1037 +2750,1037 @@
       <c r="I33" s="24"/>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="30" t="s">
+      <c r="D34" s="29"/>
+      <c r="E34" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="G34" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H34" s="30" t="s">
+      <c r="H34" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="32"/>
+      <c r="I34" s="31"/>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="30" t="s">
+      <c r="D35" s="29"/>
+      <c r="E35" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="30" t="s">
+      <c r="G35" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="30" t="s">
+      <c r="H35" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="32"/>
+      <c r="I35" s="31"/>
     </row>
     <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="30" t="s">
+      <c r="D36" s="29"/>
+      <c r="E36" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G36" s="30" t="s">
+      <c r="G36" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H36" s="30" t="s">
+      <c r="H36" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I36" s="32"/>
+      <c r="I36" s="31"/>
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="C37" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="30" t="s">
+      <c r="D37" s="29"/>
+      <c r="E37" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G37" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="30" t="s">
+      <c r="H37" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I37" s="32"/>
+      <c r="I37" s="31"/>
     </row>
     <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="30" t="s">
+      <c r="D38" s="29"/>
+      <c r="E38" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G38" s="30" t="s">
+      <c r="G38" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H38" s="30" t="s">
+      <c r="H38" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I38" s="32"/>
+      <c r="I38" s="31"/>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="30" t="s">
+      <c r="D39" s="29"/>
+      <c r="E39" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G39" s="30" t="s">
+      <c r="G39" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H39" s="30" t="s">
+      <c r="H39" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="32"/>
+      <c r="I39" s="31"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="30" t="s">
+      <c r="D40" s="29"/>
+      <c r="E40" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G40" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H40" s="30" t="s">
+      <c r="H40" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I40" s="32"/>
+      <c r="I40" s="31"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="30" t="s">
+      <c r="D41" s="29"/>
+      <c r="E41" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G41" s="30" t="s">
+      <c r="G41" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="30" t="s">
+      <c r="H41" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I41" s="32"/>
+      <c r="I41" s="31"/>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C42" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" s="30" t="s">
+      <c r="D42" s="29"/>
+      <c r="E42" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G42" s="30" t="s">
+      <c r="G42" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I42" s="32"/>
+      <c r="I42" s="31"/>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" s="30" t="s">
+      <c r="D43" s="29"/>
+      <c r="E43" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G43" s="30" t="s">
+      <c r="G43" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I43" s="32"/>
+      <c r="I43" s="31"/>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" s="30" t="s">
+      <c r="D44" s="29"/>
+      <c r="E44" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="30" t="s">
+      <c r="G44" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H44" s="30" t="s">
+      <c r="H44" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I44" s="32"/>
+      <c r="I44" s="31"/>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C45" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" s="30" t="s">
+      <c r="D45" s="29"/>
+      <c r="E45" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G45" s="30" t="s">
+      <c r="G45" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="30" t="s">
+      <c r="H45" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I45" s="32"/>
+      <c r="I45" s="31"/>
     </row>
     <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="32" t="s">
+      <c r="C46" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" s="30" t="s">
+      <c r="D46" s="29"/>
+      <c r="E46" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="30" t="s">
+      <c r="G46" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I46" s="32"/>
+      <c r="I46" s="31"/>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="32" t="s">
+      <c r="C47" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" s="30" t="s">
+      <c r="D47" s="29"/>
+      <c r="E47" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="30" t="s">
+      <c r="G47" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="30" t="s">
+      <c r="H47" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I47" s="32"/>
+      <c r="I47" s="31"/>
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="30" t="s">
+      <c r="A48" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="32" t="s">
+      <c r="C48" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="30" t="s">
+      <c r="D48" s="29"/>
+      <c r="E48" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="30" t="s">
+      <c r="G48" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H48" s="30" t="s">
+      <c r="H48" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I48" s="32"/>
+      <c r="I48" s="31"/>
     </row>
     <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="32" t="s">
+      <c r="C49" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="30" t="s">
+      <c r="D49" s="29"/>
+      <c r="E49" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G49" s="30" t="s">
+      <c r="G49" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H49" s="30" t="s">
+      <c r="H49" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I49" s="32"/>
+      <c r="I49" s="31"/>
     </row>
     <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="32" t="s">
+      <c r="C50" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" s="30" t="s">
+      <c r="D50" s="29"/>
+      <c r="E50" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G50" s="30" t="s">
+      <c r="G50" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H50" s="30" t="s">
+      <c r="H50" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I50" s="32"/>
+      <c r="I50" s="31"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="32" t="s">
+      <c r="C51" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" s="30" t="s">
+      <c r="D51" s="29"/>
+      <c r="E51" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G51" s="30" t="s">
+      <c r="G51" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H51" s="30" t="s">
+      <c r="H51" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I51" s="32"/>
+      <c r="I51" s="31"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="31" t="s">
+      <c r="B52" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C52" s="32" t="s">
+      <c r="C52" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" s="30" t="s">
+      <c r="D52" s="29"/>
+      <c r="E52" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="30" t="s">
+      <c r="G52" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H52" s="30" t="s">
+      <c r="H52" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I52" s="32"/>
+      <c r="I52" s="31"/>
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C53" s="32" t="s">
+      <c r="C53" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" s="30" t="s">
+      <c r="D53" s="29"/>
+      <c r="E53" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G53" s="30" t="s">
+      <c r="G53" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="H53" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I53" s="32"/>
+      <c r="I53" s="31"/>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
+      <c r="A54" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="31" t="s">
+      <c r="B54" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C54" s="32" t="s">
+      <c r="C54" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" s="30" t="s">
+      <c r="D54" s="29"/>
+      <c r="E54" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G54" s="30" t="s">
+      <c r="G54" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H54" s="30" t="s">
+      <c r="H54" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I54" s="32"/>
+      <c r="I54" s="31"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="31" t="s">
+      <c r="B55" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="C55" s="32" t="s">
+      <c r="C55" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" s="30" t="s">
+      <c r="D55" s="29"/>
+      <c r="E55" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G55" s="30" t="s">
+      <c r="G55" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H55" s="30" t="s">
+      <c r="H55" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I55" s="32"/>
+      <c r="I55" s="31"/>
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="30" t="s">
+      <c r="A56" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="C56" s="32" t="s">
+      <c r="C56" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" s="30" t="s">
+      <c r="D56" s="29"/>
+      <c r="E56" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G56" s="30" t="s">
+      <c r="G56" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H56" s="30" t="s">
+      <c r="H56" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I56" s="32"/>
+      <c r="I56" s="31"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+      <c r="A57" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B57" s="31" t="s">
+      <c r="B57" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="32" t="s">
+      <c r="C57" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" s="30" t="s">
+      <c r="D57" s="29"/>
+      <c r="E57" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G57" s="30" t="s">
+      <c r="G57" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H57" s="30" t="s">
+      <c r="H57" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I57" s="32"/>
+      <c r="I57" s="31"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C58" s="32" t="s">
+      <c r="C58" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" s="30" t="s">
+      <c r="D58" s="29"/>
+      <c r="E58" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G58" s="30" t="s">
+      <c r="G58" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H58" s="30" t="s">
+      <c r="H58" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I58" s="32"/>
+      <c r="I58" s="31"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="31" t="s">
+      <c r="B59" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C59" s="32" t="s">
+      <c r="C59" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" s="30" t="s">
+      <c r="D59" s="29"/>
+      <c r="E59" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G59" s="30" t="s">
+      <c r="G59" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H59" s="30" t="s">
+      <c r="H59" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I59" s="32"/>
+      <c r="I59" s="31"/>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="30" t="s">
+      <c r="A60" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="B60" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C60" s="32" t="s">
+      <c r="C60" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" s="30" t="s">
+      <c r="D60" s="29"/>
+      <c r="E60" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G60" s="30" t="s">
+      <c r="G60" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="30" t="s">
+      <c r="H60" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I60" s="32"/>
+      <c r="I60" s="31"/>
     </row>
     <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+      <c r="A61" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B61" s="31" t="s">
+      <c r="B61" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="32" t="s">
+      <c r="C61" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="30" t="s">
+      <c r="D61" s="29"/>
+      <c r="E61" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G61" s="30" t="s">
+      <c r="G61" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H61" s="30" t="s">
+      <c r="H61" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I61" s="32"/>
+      <c r="I61" s="31"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="30" t="s">
+      <c r="A62" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="31" t="s">
+      <c r="B62" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C62" s="32" t="s">
+      <c r="C62" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" s="30" t="s">
+      <c r="D62" s="29"/>
+      <c r="E62" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G62" s="30" t="s">
+      <c r="G62" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H62" s="30" t="s">
+      <c r="H62" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I62" s="32"/>
+      <c r="I62" s="31"/>
     </row>
     <row r="63" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A63" s="30" t="s">
+      <c r="A63" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B63" s="31" t="s">
+      <c r="B63" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C63" s="32" t="s">
+      <c r="C63" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F63" s="30" t="s">
+      <c r="D63" s="29"/>
+      <c r="E63" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G63" s="30" t="s">
+      <c r="G63" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H63" s="30" t="s">
+      <c r="H63" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I63" s="32"/>
+      <c r="I63" s="31"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="30" t="s">
+      <c r="A64" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B64" s="31" t="s">
+      <c r="B64" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F64" s="30" t="s">
+      <c r="D64" s="29"/>
+      <c r="E64" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G64" s="30" t="s">
+      <c r="G64" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H64" s="30" t="s">
+      <c r="H64" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I64" s="32"/>
+      <c r="I64" s="31"/>
     </row>
     <row r="65" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="s">
+      <c r="A65" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="B65" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F65" s="30" t="s">
+      <c r="D65" s="29"/>
+      <c r="E65" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G65" s="30" t="s">
+      <c r="G65" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H65" s="30" t="s">
+      <c r="H65" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I65" s="32"/>
+      <c r="I65" s="31"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="30" t="s">
+      <c r="A66" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="B66" s="31" t="s">
+      <c r="B66" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C66" s="32" t="s">
+      <c r="C66" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F66" s="30" t="s">
+      <c r="D66" s="29"/>
+      <c r="E66" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G66" s="30" t="s">
+      <c r="G66" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H66" s="30" t="s">
+      <c r="H66" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I66" s="32"/>
+      <c r="I66" s="31"/>
     </row>
     <row r="67" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A67" s="30" t="s">
+      <c r="A67" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B67" s="31" t="s">
+      <c r="B67" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C67" s="32" t="s">
+      <c r="C67" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F67" s="30" t="s">
+      <c r="D67" s="29"/>
+      <c r="E67" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G67" s="30" t="s">
+      <c r="G67" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H67" s="30" t="s">
+      <c r="H67" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I67" s="32"/>
+      <c r="I67" s="31"/>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="30" t="s">
+      <c r="A68" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B68" s="31" t="s">
+      <c r="B68" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C68" s="32" t="s">
+      <c r="C68" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F68" s="30" t="s">
+      <c r="D68" s="29"/>
+      <c r="E68" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G68" s="30" t="s">
+      <c r="G68" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H68" s="30" t="s">
+      <c r="H68" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I68" s="32"/>
+      <c r="I68" s="31"/>
     </row>
     <row r="69" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A69" s="30" t="s">
+      <c r="A69" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B69" s="31" t="s">
+      <c r="B69" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C69" s="32" t="s">
+      <c r="C69" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F69" s="30" t="s">
+      <c r="D69" s="29"/>
+      <c r="E69" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G69" s="30" t="s">
+      <c r="G69" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H69" s="30" t="s">
+      <c r="H69" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I69" s="32" t="s">
+      <c r="I69" s="31" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="30" t="s">
+      <c r="A70" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B70" s="31" t="s">
+      <c r="B70" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C70" s="32" t="s">
+      <c r="C70" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="D70" s="30" t="s">
+      <c r="D70" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="E70" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F70" s="30" t="s">
+      <c r="E70" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G70" s="30" t="s">
+      <c r="G70" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H70" s="30" t="s">
+      <c r="H70" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I70" s="32"/>
+      <c r="I70" s="31"/>
     </row>
     <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="30" t="s">
+      <c r="A71" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B71" s="31" t="s">
+      <c r="B71" s="30" t="s">
         <v>108</v>
       </c>
       <c r="C71" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="D71" s="30" t="s">
+      <c r="D71" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="E71" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F71" s="30" t="s">
+      <c r="E71" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G71" s="30" t="s">
+      <c r="G71" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H71" s="30" t="s">
+      <c r="H71" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I71" s="32"/>
+      <c r="I71" s="31"/>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="30" t="s">
+      <c r="A72" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="B72" s="31" t="s">
+      <c r="B72" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C72" s="32" t="s">
+      <c r="C72" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="D72" s="30" t="s">
+      <c r="D72" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="E72" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F72" s="30" t="s">
+      <c r="E72" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G72" s="30" t="s">
+      <c r="G72" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H72" s="30" t="s">
+      <c r="H72" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I72" s="32"/>
+      <c r="I72" s="31"/>
     </row>
     <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="s">
+      <c r="A73" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B73" s="31" t="s">
+      <c r="B73" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C73" s="32" t="s">
+      <c r="C73" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30" t="s">
+      <c r="D73" s="29"/>
+      <c r="E73" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F73" s="30" t="s">
+      <c r="F73" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G73" s="30" t="s">
+      <c r="G73" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H73" s="30" t="s">
+      <c r="H73" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I73" s="32"/>
+      <c r="I73" s="31"/>
     </row>
     <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="30" t="s">
+      <c r="A74" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B74" s="31" t="s">
+      <c r="B74" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C74" s="32" t="s">
+      <c r="C74" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30" t="s">
+      <c r="D74" s="29"/>
+      <c r="E74" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F74" s="30" t="s">
+      <c r="F74" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G74" s="30" t="s">
+      <c r="G74" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H74" s="30" t="s">
+      <c r="H74" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I74" s="32"/>
+      <c r="I74" s="31"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
@@ -3787,11 +3792,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -3799,6 +3799,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A71:B71 A20:H70 A34:I70 A72:I74 D71:I71">
@@ -3899,7 +3904,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B19:B74 B75:B76" numberStoredAsText="1"/>
+    <ignoredError sqref="B19:B74 B75:B76 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -3918,12 +3923,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -3972,6 +3971,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
@@ -3981,20 +3986,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4007,4 +3998,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-SHDACCWS] Update RS according to v20190618 document.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-SHDACCWS/MS-SHDACCWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-SHDACCWS/MS-SHDACCWS_RequirementSpecification.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A52F76-2486-4592-AA3E-C5CA8C3CEFF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -20,8 +21,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmp75D4" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmp75D4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-xiayan\AppData\Local\Temp\1\tmp75D4.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -578,16 +579,7 @@
     <t>[In Transport] Protocol servers MUST support SOAP over HTTP.</t>
   </si>
   <si>
-    <t>[In Transport] Protocol messages MUST be formatted as specified either in [SOAP1.1], Section 4, SOAP envelope or in [SOAP1.2/1],  Section 5, SOAP Message Construct.</t>
-  </si>
-  <si>
-    <t>[In Transport] Protocol server faults MUST be returned either using HTTP Status Codes as specified in [RFC2616], Section 10, Status Code Definitions, or using SOAP faults as specified either in [SOAP1.1], Section 4.4. or in [SOAP1.2/1], Section 5.4.</t>
-  </si>
-  <si>
     <t>[In Common Message Syntax] This section contains common definitions that are used by this protocol.</t>
-  </si>
-  <si>
-    <t>[In Common Message Syntax] The syntax of the definitions uses XML schema, as specified in [XMLSCHEMA1] and [XMLSCHEMA2], and WSDL, as specified in [WSDL].</t>
   </si>
   <si>
     <t>[In Namespaces] This protocol specifies and references XML namespaces using the mechanisms specified in [XMLNS].</t>
@@ -609,10 +601,6 @@
   <si>
     <t>[In Namespaces] [http] Prefix "s" is used for namesapce URI "
 http://www.w3.org/2001/XMLSchema ", reference is [XMLSCHEMA1].</t>
-  </si>
-  <si>
-    <t>[In Namespaces] [http] Prefix "soap12" is used for namespace URI "
-http://schemas.xmlsoap.org/wsdl/soap12/ ", references are [SOAP1.2/1] and [SOAP1.2/2].</t>
   </si>
   <si>
     <t>[In Namespaces] [http] Prefix "wsdl" is used for namespace URI is "
@@ -805,14 +793,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6.0</t>
+    <t>8.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Transport] Protocol messages MUST be formatted as specified either in [SOAP1.1], Section 4, SOAP envelope or in [SOAP1.2-1/2007],  Section 5, SOAP Message Construct.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Transport] Protocol server faults MUST be returned either using HTTP Status Codes as specified in [RFC2616], Section 10, Status Code Definitions, or using SOAP faults as specified either in [SOAP1.1], Section 4.4. or in [SOAP1.2-1/2007], Section 5.4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Common Message Syntax] The syntax of the definitions uses XML schema, as specified in [XMLSCHEMA1/2] and [XMLSCHEMA2/2], and WSDL, as specified in [WSDL].</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Namespaces] [http] Prefix "soap12" is used for namespace URI "
+http://schemas.xmlsoap.org/wsdl/soap12/ ", references are [SOAP1.2-1/2007] and [SOAP1.2-2/2007].</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="177" formatCode="0.0.0"/>
@@ -1079,21 +1084,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1117,6 +1107,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1694,34 +1699,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I74" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I74" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I74" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -1730,12 +1735,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2061,7 +2066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L76"/>
   <sheetViews>
@@ -2084,7 +2089,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -2094,7 +2099,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2108,138 +2113,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F3" s="12">
-        <v>42566</v>
+        <v>43634</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2252,12 +2257,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2270,12 +2275,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2288,12 +2293,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2306,60 +2311,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -2442,7 +2447,7 @@
         <v>17</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.15">
@@ -2453,10 +2458,10 @@
         <v>97</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E22" s="22" t="s">
         <v>22</v>
@@ -2471,7 +2476,7 @@
         <v>21</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -2482,7 +2487,7 @@
         <v>97</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="s">
@@ -2507,7 +2512,7 @@
         <v>97</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22" t="s">
@@ -2520,7 +2525,7 @@
         <v>15</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I24" s="24"/>
     </row>
@@ -2532,7 +2537,7 @@
         <v>98</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
@@ -2557,7 +2562,7 @@
         <v>98</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>114</v>
+        <v>172</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
@@ -2582,7 +2587,7 @@
         <v>99</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22" t="s">
@@ -2607,7 +2612,7 @@
         <v>99</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22" t="s">
@@ -2632,7 +2637,7 @@
         <v>99</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22" t="s">
@@ -2657,7 +2662,7 @@
         <v>99</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -2682,7 +2687,7 @@
         <v>99</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22" t="s">
@@ -2707,7 +2712,7 @@
         <v>99</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
@@ -2732,7 +2737,7 @@
         <v>99</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22" t="s">
@@ -2757,7 +2762,7 @@
         <v>99</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="29" t="s">
@@ -2782,7 +2787,7 @@
         <v>99</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29" t="s">
@@ -2807,7 +2812,7 @@
         <v>99</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29" t="s">
@@ -2832,7 +2837,7 @@
         <v>99</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29" t="s">
@@ -2857,7 +2862,7 @@
         <v>99</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29" t="s">
@@ -2882,7 +2887,7 @@
         <v>99</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29" t="s">
@@ -2907,7 +2912,7 @@
         <v>100</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="29" t="s">
@@ -2932,7 +2937,7 @@
         <v>100</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="29" t="s">
@@ -2949,7 +2954,7 @@
       </c>
       <c r="I41" s="31"/>
     </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
         <v>64</v>
       </c>
@@ -2957,7 +2962,7 @@
         <v>100</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="29" t="s">
@@ -2982,7 +2987,7 @@
         <v>100</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29" t="s">
@@ -3007,7 +3012,7 @@
         <v>100</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29" t="s">
@@ -3032,7 +3037,7 @@
         <v>100</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29" t="s">
@@ -3057,7 +3062,7 @@
         <v>100</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29" t="s">
@@ -3082,7 +3087,7 @@
         <v>101</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29" t="s">
@@ -3107,7 +3112,7 @@
         <v>102</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="29" t="s">
@@ -3132,7 +3137,7 @@
         <v>32</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="29" t="s">
@@ -3157,7 +3162,7 @@
         <v>32</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="29" t="s">
@@ -3182,7 +3187,7 @@
         <v>32</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D51" s="29"/>
       <c r="E51" s="29" t="s">
@@ -3207,7 +3212,7 @@
         <v>32</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D52" s="29"/>
       <c r="E52" s="29" t="s">
@@ -3232,7 +3237,7 @@
         <v>103</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="29" t="s">
@@ -3257,7 +3262,7 @@
         <v>103</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D54" s="29"/>
       <c r="E54" s="29" t="s">
@@ -3282,7 +3287,7 @@
         <v>104</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29" t="s">
@@ -3307,7 +3312,7 @@
         <v>104</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D56" s="29"/>
       <c r="E56" s="29" t="s">
@@ -3332,7 +3337,7 @@
         <v>104</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D57" s="29"/>
       <c r="E57" s="29" t="s">
@@ -3357,7 +3362,7 @@
         <v>105</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D58" s="29"/>
       <c r="E58" s="29" t="s">
@@ -3382,7 +3387,7 @@
         <v>105</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29" t="s">
@@ -3407,7 +3412,7 @@
         <v>106</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="29" t="s">
@@ -3432,7 +3437,7 @@
         <v>106</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D61" s="29"/>
       <c r="E61" s="29" t="s">
@@ -3457,7 +3462,7 @@
         <v>107</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="29" t="s">
@@ -3474,7 +3479,7 @@
       </c>
       <c r="I62" s="31"/>
     </row>
-    <row r="63" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A63" s="29" t="s">
         <v>85</v>
       </c>
@@ -3482,7 +3487,7 @@
         <v>107</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29" t="s">
@@ -3507,7 +3512,7 @@
         <v>107</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29" t="s">
@@ -3524,7 +3529,7 @@
       </c>
       <c r="I64" s="31"/>
     </row>
-    <row r="65" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="29" t="s">
         <v>87</v>
       </c>
@@ -3532,7 +3537,7 @@
         <v>107</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29" t="s">
@@ -3557,7 +3562,7 @@
         <v>108</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="29" t="s">
@@ -3582,7 +3587,7 @@
         <v>108</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29" t="s">
@@ -3607,7 +3612,7 @@
         <v>108</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -3632,7 +3637,7 @@
         <v>108</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -3648,7 +3653,7 @@
         <v>17</v>
       </c>
       <c r="I69" s="31" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3659,10 +3664,10 @@
         <v>108</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D70" s="29" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E70" s="29" t="s">
         <v>19</v>
@@ -3686,10 +3691,10 @@
         <v>108</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E71" s="29" t="s">
         <v>19</v>
@@ -3713,10 +3718,10 @@
         <v>108</v>
       </c>
       <c r="C72" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="D72" s="29" t="s">
         <v>159</v>
-      </c>
-      <c r="D72" s="29" t="s">
-        <v>163</v>
       </c>
       <c r="E72" s="29" t="s">
         <v>19</v>
@@ -3740,7 +3745,7 @@
         <v>109</v>
       </c>
       <c r="C73" s="31" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29" t="s">
@@ -3765,7 +3770,7 @@
         <v>109</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="29" t="s">
@@ -3792,6 +3797,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -3799,11 +3809,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A71:B71 A20:H70 A34:I70 A72:I74 D71:I71">
@@ -3881,20 +3886,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F74" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E74" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G74" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H74">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H74" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3904,7 +3909,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B19:B74 B75:B76 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B19:B74 B75:B76" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -3914,15 +3919,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -3971,6 +3967,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -3978,14 +3983,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3996,6 +3993,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>